<commit_message>
[UPDATE] authors data 2
</commit_message>
<xml_diff>
--- a/backend/db_mia.xlsx
+++ b/backend/db_mia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\dev\testAI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\dev\datathon2Bio\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705E0E98-B441-4CBD-88E6-14F5D7BDB95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5948D799-70C9-43B1-B0AB-90CC67265A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13550" yWindow="-800" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -3220,10 +3220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF02E344-E858-4D23-9F88-CCE308A0FAA0}">
-  <dimension ref="A1:Y40"/>
+  <dimension ref="A1:Y54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6158,6 +6158,972 @@
         <v>277</v>
       </c>
     </row>
+    <row r="41" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>3081088613</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1">
+        <v>59703800</v>
+      </c>
+      <c r="U41" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="V41" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X41" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Y41" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>1319277497</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1">
+        <v>43117360</v>
+      </c>
+      <c r="U42" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="V42" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X42" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Y42" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>1318083751</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1">
+        <v>98047360</v>
+      </c>
+      <c r="U43" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="V43" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X43" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Y43" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>4104105637</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1">
+        <v>22874010</v>
+      </c>
+      <c r="U44" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="V44" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X44" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y44" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>215875096</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1">
+        <v>90158670</v>
+      </c>
+      <c r="U45" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="V45" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X45" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y45" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>1320497570</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1">
+        <v>58567220</v>
+      </c>
+      <c r="U46" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="V46" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X46" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y46" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>2594442904</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1">
+        <v>10387670</v>
+      </c>
+      <c r="U47" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="V47" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X47" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y47" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>4406768202</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1">
+        <v>23039950</v>
+      </c>
+      <c r="U48" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="V48" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X48" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y48" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>477210473</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1">
+        <v>23053350</v>
+      </c>
+      <c r="U49" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="V49" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X49" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y49" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>4846361572</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1">
+        <v>65039210</v>
+      </c>
+      <c r="U50" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="V50" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W50" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X50" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y50" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>2442966761</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1">
+        <v>86811830</v>
+      </c>
+      <c r="U51" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="V51" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W51" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X51" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y51" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>1061114992</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1">
+        <v>85509480</v>
+      </c>
+      <c r="U52" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="V52" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X52" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y52" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>1698386522</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P53" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1">
+        <v>93902280</v>
+      </c>
+      <c r="U53" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="V53" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W53" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X53" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y53" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>1698869741</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P54" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1">
+        <v>86080330</v>
+      </c>
+      <c r="U54" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="V54" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W54" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X54" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y54" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="U5" r:id="rId1" xr:uid="{980A9992-C067-4EBF-93B5-AB1CDE56DB72}"/>
@@ -6173,980 +7139,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3FA0166-6AB1-4E60-A273-9F5F93ADEA9C}">
-  <dimension ref="A2:Y76"/>
+  <dimension ref="A16:Y76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD76"/>
+      <selection activeCell="A15" sqref="A2:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>3081088613</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1">
-        <v>59703800</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1319277497</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1">
-        <v>43117360</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1318083751</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1">
-        <v>98047360</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4104105637</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1">
-        <v>22874010</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>215875096</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1">
-        <v>90158670</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1320497570</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1">
-        <v>58567220</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>2594442904</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1">
-        <v>10387670</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>4406768202</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1">
-        <v>23039950</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>477210473</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1">
-        <v>23053350</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>4846361572</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1">
-        <v>65039210</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Y11" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>2442966761</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1">
-        <v>86811830</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1061114992</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1">
-        <v>85509480</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1698386522</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1">
-        <v>93902280</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>1698869741</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1">
-        <v>86080330</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="W15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X15" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Y15" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
     <row r="16" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1698582600</v>

</xml_diff>